<commit_message>
update project hours spreadsheet
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarno\Ohjelmointi\activity-app\front\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB05A8AA-4CB9-403F-A872-79ABFAECEF6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED75F98A-58C9-4D2F-81F7-3139AB140031}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="30588" windowHeight="16687" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>FULL STACK WEB DEVELOPMENT HARJOITUSTYÖN TUNTIKIRJANPITO</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>Strava-datan selvittelyä ja mock datan lisäilyä</t>
+  </si>
+  <si>
+    <t>24.3.2019</t>
+  </si>
+  <si>
+    <t>23.3.2019</t>
+  </si>
+  <si>
+    <t>react-bootstrap kertaus, diagrammikirjaston valinta, recharts-kirjastoon perehtyminen</t>
+  </si>
+  <si>
+    <t>activitysummary komponentin tekoa, rechartsin opiskelua</t>
   </si>
 </sst>
 </file>
@@ -127,14 +139,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,40 +462,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13" style="6" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="34.549999999999997" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="34.549999999999997" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -494,7 +506,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="58.55" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3">
@@ -505,7 +517,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29.3" x14ac:dyDescent="0.45">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3">
@@ -516,7 +528,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.3" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3">
@@ -524,6 +536,28 @@
       </c>
       <c r="C8" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.95" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.3" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add filtering by sport to activities summary
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarno\Ohjelmointi\activity-app\front\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED75F98A-58C9-4D2F-81F7-3139AB140031}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587D6CFD-5A15-41AB-ABFB-83756C13B88F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="30588" windowHeight="16687" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6409" yWindow="2983" windowWidth="18609" windowHeight="12327" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>FULL STACK WEB DEVELOPMENT HARJOITUSTYÖN TUNTIKIRJANPITO</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>activitysummary komponentin tekoa, rechartsin opiskelua</t>
+  </si>
+  <si>
+    <t>26.3.2019</t>
+  </si>
+  <si>
+    <t>TypeScript opettelua, koodin refaktorointia käyttämään paremmin TypeScriptiä, storen refaktorointia</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
@@ -560,6 +566,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="43.95" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:G1"/>

</xml_diff>

<commit_message>
add profile component, refactor
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarno\Ohjelmointi\activity-app\front\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587D6CFD-5A15-41AB-ABFB-83756C13B88F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F44079E-C81E-43BE-A71F-E66E902CC4B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6409" yWindow="2983" windowWidth="18609" windowHeight="12327" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13276" yWindow="1923" windowWidth="18610" windowHeight="12327" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>FULL STACK WEB DEVELOPMENT HARJOITUSTYÖN TUNTIKIRJANPITO</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>TypeScript opettelua, koodin refaktorointia käyttämään paremmin TypeScriptiä, storen refaktorointia</t>
+  </si>
+  <si>
+    <t>27.3.2019</t>
+  </si>
+  <si>
+    <t>profile-komponentti, refaktorointia</t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -577,6 +583,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:G1"/>

</xml_diff>

<commit_message>
add io-ts for api response validation, refactor TS types for io-ts, add activities service getAll method
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarno\Ohjelmointi\activity-app\front\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F44079E-C81E-43BE-A71F-E66E902CC4B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD09727-5F38-477A-BF35-69D046146958}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13276" yWindow="1923" windowWidth="18610" windowHeight="12327" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9463" yWindow="1978" windowWidth="18609" windowHeight="12327" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>FULL STACK WEB DEVELOPMENT HARJOITUSTYÖN TUNTIKIRJANPITO</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>profile-komponentti, refaktorointia</t>
+  </si>
+  <si>
+    <t>28.3.2019</t>
+  </si>
+  <si>
+    <t>json-server backendiin, frontin service aloitus, api vastausten TS-validoinnin selvittelyä, validointi io-ts -kirjastolla, sen opettelua, karmea määrä TS -tyyppien refaktorointia käyttämään io-ts tyyppejä</t>
   </si>
 </sst>
 </file>
@@ -474,9 +480,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -577,7 +583,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>16</v>
@@ -588,10 +594,21 @@
         <v>17</v>
       </c>
       <c r="B12" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="73.2" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated project working hours spreadsheet
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">FULL STACK WEB DEVELOPMENT HARJOITUSTYÖN TUNTIKIRJANPITO</t>
   </si>
@@ -89,7 +89,14 @@
   </si>
   <si>
     <t xml:space="preserve">- Lisätty front ja back puolelle sovelluksen oauth autorisointi Stravan API:iin käyttäjän toimesta. 
-- Korvattu json-server backend-palvelimen rungolla</t>
+- Korvattu json-server backend-palvelimen rungolla
+- Tappelua react dev serverin hot reloadin kanssa. Selvisi, että proxyn käyttäminen rikkoo reloadin jos selaimena Firefox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.8.2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend: lisätty nodemon, lisätty mongodb tietokanta, tapeltu mongoose+TS interfacet kanssa, jatkettu oauth autorisointia Strava API:iin lisäämällä access tokenien haku kun käyttäjä on antanut luvan tietojen käyttöön ja on saatu Stravan koodi tokeneita varten.</t>
   </si>
 </sst>
 </file>
@@ -236,10 +243,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -248,7 +255,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="35.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -368,7 +375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="64.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="102.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -377,6 +384,17 @@
       </c>
       <c r="C14" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update project workhours spreadsheet
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">FULL STACK WEB DEVELOPMENT HARJOITUSTYÖN TUNTIKIRJANPITO</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t xml:space="preserve">Backend: lisätty nodemon, lisätty mongodb tietokanta, tapeltu mongoose+TS interfacet kanssa, jatkettu oauth autorisointia Strava API:iin lisäämällä access tokenien haku kun käyttäjä on antanut luvan tietojen käyttöön ja on saatu Stravan koodi tokeneita varten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.8.2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Käyttäjän lisäämisen ja loginin tekoa, react-bootstrap formien ja typescript tyyppien kanssa taistelua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.8.2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Käyttäjän lisääminen ja login viimeistelty</t>
   </si>
 </sst>
 </file>
@@ -243,10 +255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -397,6 +409,28 @@
         <v>24</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="39.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:G1"/>

</xml_diff>

<commit_message>
added fetching of basic Strava activities data
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -108,7 +108,7 @@
     <t xml:space="preserve">11.8.2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Käyttäjän lisääminen ja login viimeistelty</t>
+    <t xml:space="preserve">Käyttäjän lisääminen ja login viimeistelty, Strava tokenien tallennus tietokantaan, yksinkertainen Strava aktiviteettien haku fronttiin</t>
   </si>
 </sst>
 </file>
@@ -258,7 +258,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -420,12 +420,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
improved layout, implemented refreshing of oauth tokens
</commit_message>
<xml_diff>
--- a/fitness-app-tuntikirjanpito.xlsx
+++ b/fitness-app-tuntikirjanpito.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">FULL STACK WEB DEVELOPMENT HARJOITUSTYÖN TUNTIKIRJANPITO</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t xml:space="preserve">Käyttäjän lisääminen ja login viimeistelty, Strava tokenien tallennus tietokantaan, yksinkertainen Strava aktiviteettien haku fronttiin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13. ja 14.8.2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontin ulkoasun parantelua, vanhaksi mennen Strava oauth tokenin uudistaminen</t>
   </si>
 </sst>
 </file>
@@ -255,10 +261,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,6 +437,17 @@
         <v>28</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="26.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C1:G1"/>

</xml_diff>